<commit_message>
Update after thesis submission with desktop version
</commit_message>
<xml_diff>
--- a/abbreviation.xlsx
+++ b/abbreviation.xlsx
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
-  <si>
-    <t>\textbf{ATAC-seq} &amp; \\</t>
-  </si>
-  <si>
-    <t>\textbf{Atopic dermatitis} &amp; AD \\</t>
-  </si>
-  <si>
-    <t>\textbf{ChIPm} &amp;  \\</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>\textbf{CLE} &amp; cutaneous lupus erythematosus \\</t>
   </si>
@@ -41,36 +32,24 @@
     <t>\textbf{DMARDs} &amp; disease-modifying antirheumatic drugs \\</t>
   </si>
   <si>
-    <t>\textbf{Fast-ATAC} &amp; \\</t>
-  </si>
-  <si>
     <t>\textbf{GWAS} &amp; Genome-wide association studies\\</t>
   </si>
   <si>
     <t>\textbf{NSAID} &amp; nonsteroidal antiinflammatory drug \\</t>
   </si>
   <si>
-    <t>\textbf{Omni-ATAC} &amp; \\</t>
-  </si>
-  <si>
     <t>\textbf{PI} &amp; Protein inhibitor \\</t>
   </si>
   <si>
     <t>\textbf{qPCR} &amp; quantitative polymerase chain reaction \\</t>
   </si>
   <si>
-    <t>\textbf{RA} &amp; Rheumatoid arthritis \\</t>
-  </si>
-  <si>
     <t>\textbf{ROS} &amp; Reactive oxygen species \\</t>
   </si>
   <si>
     <t>\textbf{SDS} &amp; Sodium dodecyl sulfate \\</t>
   </si>
   <si>
-    <t>\textbf{SF} &amp; Synovial fluid\\</t>
-  </si>
-  <si>
     <t>\textbf{GWAS} &amp; Genome-wide association studies \\</t>
   </si>
   <si>
@@ -80,9 +59,6 @@
     <t>\textbf{SpA} &amp; Spondyloarthritis \\</t>
   </si>
   <si>
-    <t>\textbf{NF-$\kappa$B} &amp; \\</t>
-  </si>
-  <si>
     <t>\textbf{PsA} Psoriatic arthritis&amp;  \\</t>
   </si>
   <si>
@@ -155,9 +131,6 @@
     <t>\textbf{FAIRE-seq} &amp; Formaldehyde-assisted isolation of regulatory elements sequencing \\</t>
   </si>
   <si>
-    <t>\textbf{ATAC-seq} &amp; Assay for transposase-tccessible chromatin using sequencing\\</t>
-  </si>
-  <si>
     <t>\textbf{MNase-seq} &amp; Micrococcal nuclease sequencing \\</t>
   </si>
   <si>
@@ -236,9 +209,6 @@
     <t>\textbf{SF} &amp; synovial fluid \\</t>
   </si>
   <si>
-    <t>\textbf{PB} Peripheral blood&amp; \\</t>
-  </si>
-  <si>
     <t>\textbf{NBF} &amp; Nucleosome-bound fragment\\</t>
   </si>
   <si>
@@ -252,6 +222,24 @@
   </si>
   <si>
     <t>\textbf{DAR} &amp; Differentially accessible region  \\</t>
+  </si>
+  <si>
+    <t>\textbf{AD} &amp; Atopic dermatitis \\</t>
+  </si>
+  <si>
+    <t>\textbf{ChIPm} &amp; (Chromatin immunoprecipitation)-mentation  \\</t>
+  </si>
+  <si>
+    <t>\textbf{NF-$\kappa$B} &amp; Nuclear factor kappa-light-chain-enhancer of activated B cells \\</t>
+  </si>
+  <si>
+    <t>\textbf{ATAC-seq} &amp; Assay for transposase-accessible chromatin using sequencing\\</t>
+  </si>
+  <si>
+    <t>\textbf{Fast-ATAC} &amp; Fast  assay for transposase-accessible chromatin \\</t>
+  </si>
+  <si>
+    <t>\textbf{Omni-ATAC} &amp; Omni- assay for transposase-accessible chromatin\\</t>
   </si>
 </sst>
 </file>
@@ -569,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A95"/>
+  <dimension ref="A1:A91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,402 +570,402 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
@@ -987,77 +975,57 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A80">
-    <sortCondition ref="A7"/>
+  <sortState ref="A1:A91">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>